<commit_message>
[ASE21] Add real final evaluation data
</commit_message>
<xml_diff>
--- a/eval/inspection-summary.xlsx
+++ b/eval/inspection-summary.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mini/plrg/jiset/eval/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3FA730D9-C953-5944-B4FA-DF3EE719F713}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8E704978-A95C-8943-84E2-1DB0607DF73C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1000" windowWidth="27900" windowHeight="16440"/>
+    <workbookView xWindow="17020" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inspection-summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="280" uniqueCount="86">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="263" uniqueCount="80">
   <si>
     <t>bug</t>
   </si>
@@ -94,12 +93,6 @@
     <t>E</t>
   </si>
   <si>
-    <t>[Bug] unknown variable: CatchFinallyFunctions @ Promise.prototype.finally</t>
-  </si>
-  <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>[Bug] unknown variable: obj @ Array.prototype.sort</t>
   </si>
   <si>
@@ -190,18 +183,12 @@
     <t>[Bug] unchecked abrupt completions: alreadyDeclared @ FunctionDeclarationInstantiation</t>
   </si>
   <si>
-    <t>[Bug] unknown variable: PromiseRejectFunctions @ CreateResolvingFunctions</t>
-  </si>
-  <si>
     <t>[Bug] unchecked abrupt completions: V @ CreateDataProperty</t>
   </si>
   <si>
     <t>[Bug] non-numeric types: argument @ IsNonNegativeInteger</t>
   </si>
   <si>
-    <t>[Bug] unknown variable: stepsReject @ CreateResolvingFunctions</t>
-  </si>
-  <si>
     <t>[Bug] assertion failed: (= (typeof O) Object) @ DefinePropertyOrThrow</t>
   </si>
   <si>
@@ -253,9 +240,6 @@
     <t>[Bug] assertion failed: (= MultiplicativeOperator "%") @ MultiplicativeExpression[1,0].Evaluation</t>
   </si>
   <si>
-    <t>[Bug] unknown variable: stepsCatchFinally @ Promise.prototype.finally</t>
-  </si>
-  <si>
     <t>[Bug] assertion failed: false @ ToBoolean</t>
   </si>
   <si>
@@ -272,10 +256,6 @@
   </si>
   <si>
     <t>[Bug] unchecked abrupt completions: lref.ReferencedName @ AssignmentExpression[6,0].Evaluation</t>
-  </si>
-  <si>
-    <t>TODO</t>
-    <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>R</t>
@@ -293,7 +273,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19">
     <font>
       <sz val="12"/>
@@ -1238,11 +1218,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F69"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1281,10 +1261,10 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F2">
-        <f>COUNTIF($D$2:$D$69, E2)</f>
+        <f>COUNTIF($D$2:$D$65, E2)</f>
         <v>19</v>
       </c>
     </row>
@@ -1302,10 +1282,10 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F3">
-        <f>COUNTIF($D$2:$D$69, E3)</f>
+        <f>COUNTIF($D$2:$D$65, E3)</f>
         <v>28</v>
       </c>
     </row>
@@ -1323,10 +1303,10 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F4">
-        <f>COUNTIF($D$2:$D$69, E4)</f>
+        <f>COUNTIF($D$2:$D$65, E4)</f>
         <v>17</v>
       </c>
     </row>
@@ -1343,13 +1323,6 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5">
-        <f>COUNTIF($D$2:$D$69, E5)</f>
-        <v>4</v>
-      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
@@ -1366,7 +1339,7 @@
       </c>
       <c r="F6">
         <f>SUM(F2:F5)</f>
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1450,35 +1423,35 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1497,16 +1470,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1514,60 +1487,60 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -1581,49 +1554,49 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
@@ -1632,18 +1605,18 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -1651,7 +1624,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -1665,21 +1638,21 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -1688,12 +1661,12 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
@@ -1707,35 +1680,35 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
@@ -1749,91 +1722,91 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D35" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
@@ -1847,7 +1820,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
@@ -1861,41 +1834,41 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D42" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -1903,21 +1876,21 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
@@ -1926,18 +1899,18 @@
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -1945,7 +1918,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
@@ -1954,12 +1927,12 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B49" t="s">
         <v>5</v>
@@ -1973,13 +1946,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
@@ -1987,27 +1960,27 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C52" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
@@ -2015,41 +1988,41 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D53" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D54" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B55" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -2057,27 +2030,27 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D56" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B57" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D57" t="s">
         <v>21</v>
@@ -2085,27 +2058,27 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D58" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -2113,21 +2086,21 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B60" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B61" t="s">
         <v>19</v>
@@ -2141,113 +2114,57 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D62" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B63" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D63" t="s">
-        <v>82</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D64" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D65" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" t="s">
-        <v>78</v>
-      </c>
-      <c r="B66" t="s">
-        <v>8</v>
-      </c>
-      <c r="C66" t="s">
-        <v>9</v>
-      </c>
-      <c r="D66" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" t="s">
-        <v>79</v>
-      </c>
-      <c r="B67" t="s">
-        <v>8</v>
-      </c>
-      <c r="C67" t="s">
-        <v>9</v>
-      </c>
-      <c r="D67" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" t="s">
-        <v>80</v>
-      </c>
-      <c r="B68" t="s">
-        <v>19</v>
-      </c>
-      <c r="C68" t="s">
-        <v>20</v>
-      </c>
-      <c r="D68" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" t="s">
-        <v>81</v>
-      </c>
-      <c r="B69" t="s">
-        <v>8</v>
-      </c>
-      <c r="C69" t="s">
-        <v>9</v>
-      </c>
-      <c r="D69" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2255,17 +2172,4 @@
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
-  <sheetData/>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>